<commit_message>
JQuery 2.1 and NAV BAR
</commit_message>
<xml_diff>
--- a/resources/Repository Setup.xlsx
+++ b/resources/Repository Setup.xlsx
@@ -16000,8 +16000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2677" workbookViewId="0">
-      <selection activeCell="C2710" sqref="C2710"/>
+    <sheetView tabSelected="1" topLeftCell="A1037" workbookViewId="0">
+      <selection activeCell="E1070" sqref="E1070:E1076"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34200,7 +34200,7 @@
         <v>2144</v>
       </c>
       <c r="E1070" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1071" spans="1:5" x14ac:dyDescent="0.25">
@@ -34216,8 +34216,8 @@
       <c r="D1071" t="s">
         <v>2144</v>
       </c>
-      <c r="E1071" t="b">
-        <v>1</v>
+      <c r="E1071" s="25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="1072" spans="1:5" x14ac:dyDescent="0.25">
@@ -34233,8 +34233,8 @@
       <c r="D1072" t="s">
         <v>2144</v>
       </c>
-      <c r="E1072" t="b">
-        <v>1</v>
+      <c r="E1072" s="25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="1073" spans="1:5" x14ac:dyDescent="0.25">
@@ -34250,8 +34250,8 @@
       <c r="D1073" t="s">
         <v>2144</v>
       </c>
-      <c r="E1073" t="b">
-        <v>1</v>
+      <c r="E1073" s="25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="1074" spans="1:5" x14ac:dyDescent="0.25">
@@ -34267,8 +34267,8 @@
       <c r="D1074" t="s">
         <v>2144</v>
       </c>
-      <c r="E1074" t="b">
-        <v>1</v>
+      <c r="E1074" s="25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="1075" spans="1:5" x14ac:dyDescent="0.25">
@@ -34284,8 +34284,8 @@
       <c r="D1075" t="s">
         <v>2144</v>
       </c>
-      <c r="E1075" t="b">
-        <v>1</v>
+      <c r="E1075" s="25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="1076" spans="1:5" x14ac:dyDescent="0.25">
@@ -34301,8 +34301,8 @@
       <c r="D1076" t="s">
         <v>2144</v>
       </c>
-      <c r="E1076" t="b">
-        <v>1</v>
+      <c r="E1076" s="25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="1077" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Lot of changes and wizard creation not working
</commit_message>
<xml_diff>
--- a/resources/Repository Setup.xlsx
+++ b/resources/Repository Setup.xlsx
@@ -272,7 +272,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9702" uniqueCount="4760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9747" uniqueCount="4784">
   <si>
     <t>identifier</t>
   </si>
@@ -14521,6 +14521,9 @@
     <t>Custom list</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>status.type</t>
   </si>
   <si>
@@ -14552,6 +14555,75 @@
   </si>
   <si>
     <t>field_label</t>
+  </si>
+  <si>
+    <t>attached_account.aliases</t>
+  </si>
+  <si>
+    <t>frequency_reference.name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>owner.name</t>
+  </si>
+  <si>
+    <t>owner_role.name</t>
+  </si>
+  <si>
+    <t>parent_security</t>
+  </si>
+  <si>
+    <t>security_type.name</t>
+  </si>
+  <si>
+    <t>short_description</t>
+  </si>
+  <si>
+    <t>status.name</t>
+  </si>
+  <si>
+    <t>type.name</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>Closing date</t>
+  </si>
+  <si>
+    <t>Account aliases</t>
+  </si>
+  <si>
+    <t>Frequency reference</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>Market sector</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Owner role</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Security type</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -56833,16 +56905,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -56850,21 +56922,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4758</v>
+        <v>4759</v>
       </c>
       <c r="C1" t="s">
-        <v>4759</v>
+        <v>4760</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4749</v>
+        <v>4750</v>
       </c>
       <c r="B2" t="s">
-        <v>4753</v>
+        <v>4754</v>
       </c>
       <c r="C2" t="s">
-        <v>4754</v>
+        <v>4755</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -56872,29 +56944,29 @@
         <v>2529</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>4753</v>
+        <v>4754</v>
       </c>
       <c r="C3" t="s">
-        <v>4755</v>
+        <v>4756</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4750</v>
+        <v>4751</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>4753</v>
+        <v>4754</v>
       </c>
       <c r="C4" t="s">
-        <v>4756</v>
+        <v>4757</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4751</v>
+        <v>4752</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>4753</v>
+        <v>4754</v>
       </c>
       <c r="C5" t="s">
         <v>4051</v>
@@ -56902,16 +56974,182 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4752</v>
+        <v>4753</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>4753</v>
+        <v>4754</v>
       </c>
       <c r="C6" t="s">
-        <v>4757</v>
+        <v>4758</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4771</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>2636</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4772</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>4761</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4773</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>4762</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4774</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>4763</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4775</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>2112</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4776</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>4764</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4777</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>4765</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4778</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>4766</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4779</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>2111</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4780</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>4767</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4781</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>4768</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4782</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>4769</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4749</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>4770</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>4754</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4783</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>